<commit_message>
Adding reject reasons to reasons.ts
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -1,41 +1,332 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repository\clone_puppeteer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA57431-D61A-4656-9788-5D10DD74E8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$90</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
+  <si>
+    <t>Tracking Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>707086481688</t>
+  </si>
+  <si>
+    <t>DENIED - DOES NOT MEET ELIGIBILITY CRITERIA</t>
+  </si>
+  <si>
+    <t>273129697366</t>
+  </si>
+  <si>
+    <t>DENIED - OT ON-TIME DELIVERY</t>
+  </si>
+  <si>
+    <t>273128938174</t>
+  </si>
+  <si>
+    <t>PENDING - UNABLE TO PROCESS REQUEST</t>
+  </si>
+  <si>
+    <t>PENDING - UNABLE TO PROCESS REQUEST (THANK YOU)</t>
+  </si>
+  <si>
+    <t>273151439944</t>
+  </si>
+  <si>
+    <t>273129785744</t>
+  </si>
+  <si>
+    <t>Page didn't load.</t>
+  </si>
+  <si>
+    <t>775655598849</t>
+  </si>
+  <si>
+    <t>273026504088</t>
+  </si>
+  <si>
+    <t>273142824904</t>
+  </si>
+  <si>
+    <t>APPROVED</t>
+  </si>
+  <si>
+    <t>273327498110</t>
+  </si>
+  <si>
+    <t>273359387343</t>
+  </si>
+  <si>
+    <t>273359933604</t>
+  </si>
+  <si>
+    <t>273453193050</t>
+  </si>
+  <si>
+    <t>273299237108</t>
+  </si>
+  <si>
+    <t>273299765134</t>
+  </si>
+  <si>
+    <t>273317848435</t>
+  </si>
+  <si>
+    <t>730488063462</t>
+  </si>
+  <si>
+    <t>730488063484</t>
+  </si>
+  <si>
+    <t>707086479770</t>
+  </si>
+  <si>
+    <t>707086480096</t>
+  </si>
+  <si>
+    <t>707086481070</t>
+  </si>
+  <si>
+    <t>707086481107</t>
+  </si>
+  <si>
+    <t>707086481129</t>
+  </si>
+  <si>
+    <t>707086481232</t>
+  </si>
+  <si>
+    <t>707086481287</t>
+  </si>
+  <si>
+    <t>707086481302</t>
+  </si>
+  <si>
+    <t>707086481324</t>
+  </si>
+  <si>
+    <t>707086481335</t>
+  </si>
+  <si>
+    <t>707086481368</t>
+  </si>
+  <si>
+    <t>707086481379</t>
+  </si>
+  <si>
+    <t>707086481460</t>
+  </si>
+  <si>
+    <t>707086481471</t>
+  </si>
+  <si>
+    <t>707086481482</t>
+  </si>
+  <si>
+    <t>707086481493</t>
+  </si>
+  <si>
+    <t>707086481508</t>
+  </si>
+  <si>
+    <t>707086481519</t>
+  </si>
+  <si>
+    <t>707086481520</t>
+  </si>
+  <si>
+    <t>707086481530</t>
+  </si>
+  <si>
+    <t>707086481541</t>
+  </si>
+  <si>
+    <t>707086481552</t>
+  </si>
+  <si>
+    <t>707086481563</t>
+  </si>
+  <si>
+    <t>707086481574</t>
+  </si>
+  <si>
+    <t>707086481725</t>
+  </si>
+  <si>
+    <t>707086481736</t>
+  </si>
+  <si>
+    <t>707086482607</t>
+  </si>
+  <si>
+    <t>707086482754</t>
+  </si>
+  <si>
+    <t>726491930024</t>
+  </si>
+  <si>
+    <t>651956631206</t>
+  </si>
+  <si>
+    <t>727534459294</t>
+  </si>
+  <si>
+    <t>727534459651</t>
+  </si>
+  <si>
+    <t>775866025327</t>
+  </si>
+  <si>
+    <t>775811347058</t>
+  </si>
+  <si>
+    <t>272461530276</t>
+  </si>
+  <si>
+    <t>272684815866</t>
+  </si>
+  <si>
+    <t>272680290080</t>
+  </si>
+  <si>
+    <t>273204210432</t>
+  </si>
+  <si>
+    <t>273184588215</t>
+  </si>
+  <si>
+    <t>273192253909</t>
+  </si>
+  <si>
+    <t>720266537700</t>
+  </si>
+  <si>
+    <t>273302078341</t>
+  </si>
+  <si>
+    <t>273297047350</t>
+  </si>
+  <si>
+    <t>273296634876</t>
+  </si>
+  <si>
+    <t>720266531415</t>
+  </si>
+  <si>
+    <t>720266531805</t>
+  </si>
+  <si>
+    <t>720315971205</t>
+  </si>
+  <si>
+    <t>720315971720</t>
+  </si>
+  <si>
+    <t>720315972782</t>
+  </si>
+  <si>
+    <t>720266537365</t>
+  </si>
+  <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>720266537468</t>
+  </si>
+  <si>
+    <t>273130301207</t>
+  </si>
+  <si>
+    <t>273173268696</t>
+  </si>
+  <si>
+    <t>720315973057</t>
+  </si>
+  <si>
+    <t>775891337124</t>
+  </si>
+  <si>
+    <t>775934406352</t>
+  </si>
+  <si>
+    <t>272794816410</t>
+  </si>
+  <si>
+    <t>DENIED - 1048 CUSTOMER NOT ELIGIBLE FOR MBG</t>
+  </si>
+  <si>
+    <t>273073482556</t>
+  </si>
+  <si>
+    <t>273073484868</t>
+  </si>
+  <si>
+    <t>273292812768</t>
+  </si>
+  <si>
+    <t>732596092223</t>
+  </si>
+  <si>
+    <t>732596097567</t>
+  </si>
+  <si>
+    <t>730855700959</t>
+  </si>
+  <si>
+    <t>730855708949</t>
+  </si>
+  <si>
+    <t>730855709875</t>
+  </si>
+  <si>
+    <t>730855710033</t>
+  </si>
+  <si>
+    <t>730855710125</t>
+  </si>
+  <si>
+    <t>730855710136</t>
+  </si>
+  <si>
+    <t>735127596091</t>
+  </si>
+  <si>
+    <t>730443225200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENIED - 08 RECIPIENT NOT IN / BUSINESS CLOSED </t>
+  </si>
+  <si>
+    <t>734365153422</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +363,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,55 +695,751 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J112" sqref="J112"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Tracking Number</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Description</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>720266531415</v>
-      </c>
-      <c r="B2" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>720266531805</v>
-      </c>
-      <c r="B3" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>720315971205</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>720315971720</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PENDING - UNABLE TO PROCESS REQUEST</v>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>96</v>
+      </c>
+      <c r="B89" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>98</v>
+      </c>
+      <c r="B90" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B90" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="undefined"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
+    <ignoredError sqref="A1:B90" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>